<commit_message>
DONE: modified test plan
</commit_message>
<xml_diff>
--- a/ABU test plan.xlsx
+++ b/ABU test plan.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rconstantin\PycharmProjects\ConnectorsAsembly\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cristi\PycharmProjects\AssemblyConnector\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19560" windowHeight="8340"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$20</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="77">
   <si>
     <t>Requirements</t>
   </si>
@@ -41,15 +41,9 @@
     <t>Test(s)</t>
   </si>
   <si>
-    <t>How to do this? Check the log file? Maybe it is possible to check of phrase “&lt;name_file&gt; is”, which appears when a given arxml file is parsed and checked</t>
-  </si>
-  <si>
     <t>Check if the input and output directory are configurable</t>
   </si>
   <si>
-    <t>Call tool with a given set of input&amp;output directories and check if the output directory is created</t>
-  </si>
-  <si>
     <t>Check the encoding and namespace of the generated file</t>
   </si>
   <si>
@@ -59,9 +53,6 @@
     <t>not done</t>
   </si>
   <si>
-    <t>see TRS.ALADDIN.GEN.004 (below)</t>
-  </si>
-  <si>
     <t>done</t>
   </si>
   <si>
@@ -142,6 +133,29 @@
         <scheme val="minor"/>
       </rPr>
       <t>: feed to the tool an input file which contains two Pports referencing the same interface, and one Rport referencing the same interface referenced by the Pports.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test 2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: feed to the tool an input file which contains two PRPorts referencing the same interface, and one Rport referencing the same interface referenced by the Pports.</t>
     </r>
   </si>
   <si>
@@ -302,6 +316,29 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t>Test 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: feed to the tool one Pport and one Rport referencing an interface CS_Name1, and one Pport and one Rport referencing an interface NV_Name1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Test 2</t>
     </r>
     <r>
@@ -316,6 +353,29 @@
     </r>
   </si>
   <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: feed to the tool one Pport and one Rport referencing the same interface</t>
+    </r>
+  </si>
+  <si>
     <t>- check that the connector is created between the Pport and Rport</t>
   </si>
   <si>
@@ -412,6 +472,29 @@
     </r>
   </si>
   <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: feed to the tool one Port referencing one interface of type Client-Server and one Rport referencing the same Client-Server interface</t>
+    </r>
+  </si>
+  <si>
     <t>- check that only one connector is created between the given ports</t>
   </si>
   <si>
@@ -441,6 +524,9 @@
     </r>
   </si>
   <si>
+    <t>Test 2: feed to the tool one PRPort referencing one interface of type Client-Server, and one Rport referencing the samei Client-Server interface</t>
+  </si>
+  <si>
     <t>- check that one connector is created between the PRPort and the Rport</t>
   </si>
   <si>
@@ -475,8 +561,14 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>: feed to the tool one PRPort referencing one interface of type Client-Server, and one Rport referencing the samei Client-Server interface</t>
-    </r>
+      <t>: feed to the tool one Pport and one Rport referencing an interface CS_Name1, and one Pport and one Rport referencing an interface NV_Name2</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">- check that two connectors are created, one between the Pport o and Rport of NV_Name2, and the other between the Rport and the Pport of CS_Name1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - check in the log that all the input .arxml files are parsed</t>
   </si>
   <si>
     <r>
@@ -488,21 +580,18 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Test 2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: feed to the tool one PPort referencing one interface of type Client-Server and one Rport referencing the same Client-Server interface</t>
-    </r>
-  </si>
-  <si>
-    <t>-check that the output file does not contains multiple times the same connector</t>
+      <t>Test 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: provide to the tool several .arxml  files as an input argument</t>
+    </r>
   </si>
   <si>
     <r>
@@ -524,60 +613,20 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>: feed to the tool one Pport and one Rport referencing the same interface of type Sender-Receiver</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Test 1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: feed to the tool one Pport and one Rport referencing an interface SR_Name1, and one Pport and one Rport referencing an interface NV_Name1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Test 2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: feed to the tool an input file which contains two PRPorts referencing the same interface, and one Rport referencing the same interface referenced by the PRPports.</t>
-    </r>
+      <t>: Call tool with a given set of input&amp;output directories and check if the output directory is created</t>
+    </r>
+  </si>
+  <si>
+    <t>- check that the output folder is present</t>
+  </si>
+  <si>
+    <t>n/a</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -595,27 +644,15 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="13">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -721,7 +758,60 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right/>
@@ -761,7 +851,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -781,16 +871,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -803,59 +914,53 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="8">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -873,6 +978,26 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1191,438 +1316,442 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H7" sqref="H7"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="48.85546875" style="15" customWidth="1"/>
+    <col min="1" max="1" width="26.28515625" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.85546875" style="23" customWidth="1"/>
     <col min="3" max="3" width="79.140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="46.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" style="7" customWidth="1"/>
-    <col min="6" max="6" width="10" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" style="8" customWidth="1"/>
+    <col min="6" max="6" width="10" style="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="21" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>13</v>
+      <c r="A2" s="9" t="s">
+        <v>10</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="C4" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="20" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="27"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="20" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="20" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A12" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="35"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="20" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" s="20" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="27"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" s="20" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="20" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" s="20" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A18" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="13" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="C5" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="D5" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="20"/>
-      <c r="B6" s="21"/>
-      <c r="C6" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="D6" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="C7" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="D7" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="21"/>
-      <c r="B8" s="25"/>
-      <c r="C8" s="23" t="s">
+      <c r="B18" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="D8" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="C9" s="23" t="s">
-        <v>59</v>
-      </c>
-      <c r="D9" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="C10" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="D10" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="C11" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="D11" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="C12" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="D12" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12" s="13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A13" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="C13" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="D13" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" s="13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="17" t="s">
+    </row>
+    <row r="19" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A19" s="31"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" s="20" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="C14" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="D14" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14" s="13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="21"/>
-      <c r="B15" s="25"/>
-      <c r="C15" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="D15" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F15" s="13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" s="27" t="s">
-        <v>38</v>
-      </c>
-      <c r="D16" s="28" t="s">
-        <v>40</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F16" s="13" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" s="27" t="s">
+      <c r="C20" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="27" t="s">
-        <v>38</v>
-      </c>
-      <c r="D17" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F17" s="13" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A18" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="D18" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F18" s="13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A19" s="21"/>
-      <c r="B19" s="21"/>
-      <c r="C19" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="D19" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F19" s="13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" s="17" t="s">
+      <c r="D20" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="D20" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F20" s="13" t="s">
-        <v>67</v>
+      <c r="E20" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F20" s="20" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="30"/>
-      <c r="B21" s="30"/>
-      <c r="C21" s="23" t="s">
-        <v>73</v>
-      </c>
-      <c r="D21" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F21" s="13" t="s">
-        <v>67</v>
+      <c r="B21" s="28"/>
+      <c r="C21" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21" s="20" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="30"/>
-      <c r="B22" s="30"/>
-      <c r="C22" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="D22" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="E22" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F22" s="13" t="s">
-        <v>67</v>
+      <c r="A22" s="31"/>
+      <c r="B22" s="25"/>
+      <c r="C22" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F22" s="20" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E20" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:E20"/>
   <mergeCells count="10">
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="A5:A6"/>
@@ -1632,32 +1761,32 @@
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="A12:A13"/>
   </mergeCells>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>"not done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F22">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F22">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"YES"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E22" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E22">
       <formula1>"done, not done"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F22" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F22">
       <formula1>"YES, NO"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
DONE: completed test plan
</commit_message>
<xml_diff>
--- a/ABU test plan.xlsx
+++ b/ABU test plan.xlsx
@@ -1,25 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rconstantin\PycharmProjects\ConnectorsAsembly\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-15" yWindow="5940" windowWidth="19260" windowHeight="6000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$20</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$21</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -27,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="77">
   <si>
     <t>Requirements</t>
   </si>
@@ -41,27 +36,15 @@
     <t>Test(s)</t>
   </si>
   <si>
-    <t>How to do this? Check the log file? Maybe it is possible to check of phrase “&lt;name_file&gt; is”, which appears when a given arxml file is parsed and checked</t>
-  </si>
-  <si>
     <t>Check if the input and output directory are configurable</t>
   </si>
   <si>
-    <t>Call tool with a given set of input&amp;output directories and check if the output directory is created</t>
-  </si>
-  <si>
     <t>Check the encoding and namespace of the generated file</t>
   </si>
   <si>
     <t>Result</t>
   </si>
   <si>
-    <t>not done</t>
-  </si>
-  <si>
-    <t>see TRS.ALADDIN.GEN.004 (below)</t>
-  </si>
-  <si>
     <t>done</t>
   </si>
   <si>
@@ -142,6 +125,29 @@
         <scheme val="minor"/>
       </rPr>
       <t>: feed to the tool an input file which contains two Pports referencing the same interface, and one Rport referencing the same interface referenced by the Pports.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test 2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: feed to the tool an input file which contains two PRPorts referencing the same interface, and one Rport referencing the same interface referenced by the Pports.</t>
     </r>
   </si>
   <si>
@@ -302,6 +308,29 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t>Test 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: feed to the tool one Pport and one Rport referencing an interface CS_Name1, and one Pport and one Rport referencing an interface NV_Name1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Test 2</t>
     </r>
     <r>
@@ -316,6 +345,29 @@
     </r>
   </si>
   <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: feed to the tool one Pport and one Rport referencing the same interface</t>
+    </r>
+  </si>
+  <si>
     <t>- check that the connector is created between the Pport and Rport</t>
   </si>
   <si>
@@ -412,6 +464,29 @@
     </r>
   </si>
   <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: feed to the tool one Port referencing one interface of type Client-Server and one Rport referencing the same Client-Server interface</t>
+    </r>
+  </si>
+  <si>
     <t>- check that only one connector is created between the given ports</t>
   </si>
   <si>
@@ -450,9 +525,6 @@
     <t>passed</t>
   </si>
   <si>
-    <t>NO</t>
-  </si>
-  <si>
     <t>YES</t>
   </si>
   <si>
@@ -475,110 +547,122 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t>: feed to the tool one Pport and one Rport referencing an interface CS_Name1, and one Pport and one Rport referencing an interface NV_Name2</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">- check that two connectors are created, one between the Pport o and Rport of NV_Name2, and the other between the Rport and the Pport of CS_Name1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - check in the log that all the input .arxml files are parsed</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: provide to the tool several .arxml  files as an input argument</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Call tool with a given set of input&amp;output directories and check if the output directory is created</t>
+    </r>
+  </si>
+  <si>
+    <t>- check that the output folder is present</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test 2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: feed to the tool one Port referencing one interface of type Client-Server and one Rport referencing the same Client-Server interface</t>
+    </r>
+  </si>
+  <si>
+    <t>-check that the output file does not contains multiple times the same connector</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test 2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>: feed to the tool one PRPort referencing one interface of type Client-Server, and one Rport referencing the samei Client-Server interface</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Test 2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: feed to the tool one PPort referencing one interface of type Client-Server and one Rport referencing the same Client-Server interface</t>
-    </r>
-  </si>
-  <si>
-    <t>-check that the output file does not contains multiple times the same connector</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Test 1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: feed to the tool one Pport and one Rport referencing the same interface of type Sender-Receiver</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Test 1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: feed to the tool one Pport and one Rport referencing an interface SR_Name1, and one Pport and one Rport referencing an interface NV_Name1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Test 2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: feed to the tool an input file which contains two PRPorts referencing the same interface, and one Rport referencing the same interface referenced by the PRPports.</t>
     </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -595,27 +679,15 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="13">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -721,7 +793,60 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right/>
@@ -761,7 +886,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -781,16 +906,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -803,79 +949,56 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -972,7 +1095,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1007,7 +1130,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1184,45 +1307,45 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H7" sqref="H7"/>
+      <selection pane="bottomRight" activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="48.85546875" style="15" customWidth="1"/>
+    <col min="1" max="1" width="26.28515625" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.85546875" style="23" customWidth="1"/>
     <col min="3" max="3" width="79.140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="46.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" style="7" customWidth="1"/>
-    <col min="6" max="6" width="10" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" style="8" customWidth="1"/>
+    <col min="6" max="6" width="10" style="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:6">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="21" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>64</v>
@@ -1231,433 +1354,455 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>13</v>
+    <row r="2" spans="1:6" ht="30">
+      <c r="A2" s="9" t="s">
+        <v>9</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="30">
+      <c r="A4" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="C4" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="30">
+      <c r="A5" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="20" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="30">
+      <c r="A6" s="28"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="20" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="30">
+      <c r="A7" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="20" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="30">
+      <c r="A8" s="36"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="45">
+      <c r="A9" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="45">
+      <c r="A10" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="45">
+      <c r="A11" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="45">
+      <c r="A12" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="75">
+      <c r="A13" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="20" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="60">
+      <c r="A14" s="36"/>
+      <c r="B14" s="34"/>
+      <c r="C14" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" s="20" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="45">
+      <c r="A15" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" s="20" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="45">
+      <c r="A16" s="28"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" s="20" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="30">
+      <c r="A17" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" s="20" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="10" customFormat="1" ht="30">
+      <c r="A18" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" s="20" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="60">
+      <c r="A19" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19" s="20" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="60">
+      <c r="A20" s="32"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" s="20" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="45">
+      <c r="A21" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="13" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="C5" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="D5" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="20"/>
-      <c r="B6" s="21"/>
-      <c r="C6" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="D6" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="C7" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="D7" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="21"/>
-      <c r="B8" s="25"/>
-      <c r="C8" s="23" t="s">
-        <v>69</v>
-      </c>
-      <c r="D8" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="C9" s="23" t="s">
-        <v>59</v>
-      </c>
-      <c r="D9" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="C10" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="D10" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="C11" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="D11" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="C12" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="D12" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12" s="13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A13" s="23" t="s">
+      <c r="B21" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="C13" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="D13" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" s="13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="17" t="s">
+      <c r="C21" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="C14" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="D14" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14" s="13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="21"/>
-      <c r="B15" s="25"/>
-      <c r="C15" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="D15" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F15" s="13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" s="27" t="s">
-        <v>38</v>
-      </c>
-      <c r="D16" s="28" t="s">
-        <v>40</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F16" s="13" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" s="27" t="s">
+      <c r="D21" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F21" s="20" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="45">
+      <c r="A22" s="31"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="27" t="s">
-        <v>38</v>
-      </c>
-      <c r="D17" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F17" s="13" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A18" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" s="17" t="s">
+      <c r="D22" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="D18" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F18" s="13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A19" s="21"/>
-      <c r="B19" s="21"/>
-      <c r="C19" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="D19" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F19" s="13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" s="17" t="s">
+      <c r="E22" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22" s="20" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="45">
+      <c r="A23" s="32"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="D20" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F20" s="13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="30"/>
-      <c r="B21" s="30"/>
-      <c r="C21" s="23" t="s">
-        <v>73</v>
-      </c>
-      <c r="D21" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F21" s="13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="30"/>
-      <c r="B22" s="30"/>
-      <c r="C22" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="D22" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="E22" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F22" s="13" t="s">
-        <v>67</v>
+      <c r="D23" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F23" s="20" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E20" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <mergeCells count="10">
+  <autoFilter ref="A1:E21"/>
+  <mergeCells count="12">
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B7:B8"/>
     <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
   </mergeCells>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>"not done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F22">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+  <conditionalFormatting sqref="F2:F23">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F22">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+  <conditionalFormatting sqref="F2:F23">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"YES"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E22" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E23">
       <formula1>"done, not done"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F22" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F23">
       <formula1>"YES, NO"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Test plan: minor changes
</commit_message>
<xml_diff>
--- a/ABU test plan.xlsx
+++ b/ABU test plan.xlsx
@@ -9,15 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="5940" windowWidth="19260" windowHeight="6000"/>
+    <workbookView xWindow="-15" yWindow="5940" windowWidth="19260" windowHeight="6000" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Overview" sheetId="1" r:id="rId1"/>
+    <sheet name="Version" sheetId="3" r:id="rId1"/>
+    <sheet name="Overview" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Overview!$A$1:$E$21</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Overview!$A$1:$E$21</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="81">
   <si>
     <t>Requirements</t>
   </si>
@@ -54,51 +55,6 @@
   </si>
   <si>
     <t>covered by the tests below</t>
-  </si>
-  <si>
-    <t>TRS.ABU.INOUT.001</t>
-  </si>
-  <si>
-    <t>TRS.ABU.INOUT.100</t>
-  </si>
-  <si>
-    <t>TRS.ABU.GEN.001</t>
-  </si>
-  <si>
-    <t>TRS.ABU.GEN.002</t>
-  </si>
-  <si>
-    <t>TRS.ABU.GEN.003</t>
-  </si>
-  <si>
-    <t>TRS.ABU.GEN.004</t>
-  </si>
-  <si>
-    <t>TRS.ABU.FUNC.0001</t>
-  </si>
-  <si>
-    <t>TRS.ABU.FUNC.0002</t>
-  </si>
-  <si>
-    <t>TRS.ABU.FUNC.0003</t>
-  </si>
-  <si>
-    <t>TRS.ABU.FUNC.0004</t>
-  </si>
-  <si>
-    <t>TRS.ABU.FUNC.0005</t>
-  </si>
-  <si>
-    <t>TRS.ABU.FUNC.0006</t>
-  </si>
-  <si>
-    <t>TRS.ABU.FUNC.0007</t>
-  </si>
-  <si>
-    <t>TRS.ABU.FUNC.0008</t>
-  </si>
-  <si>
-    <t>TRS.ABU.FUNC.0009</t>
   </si>
   <si>
     <t>Check the structure of an AssemblyConnector element</t>
@@ -661,6 +617,64 @@
   </si>
   <si>
     <t>Passed</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>1.0</t>
+  </si>
+  <si>
+    <t>- initial creation 
+- created tests for ConnectorDescriptor tool V1 (delivery on 16.03.2018)</t>
+  </si>
+  <si>
+    <t>TRS.CONNECTOR.INOUT.001</t>
+  </si>
+  <si>
+    <t>TRS.CONNECTOR.INOUT.100</t>
+  </si>
+  <si>
+    <t>TRS.CONNECTOR.FUNC.0001</t>
+  </si>
+  <si>
+    <t>TRS.CONNECTOR.FUNC.0002</t>
+  </si>
+  <si>
+    <t>TRS.CONNECTOR.FUNC.0003</t>
+  </si>
+  <si>
+    <t>TRS.CONNECTOR.FUNC.0004</t>
+  </si>
+  <si>
+    <t>TRS.CONNECTOR.FUNC.0005</t>
+  </si>
+  <si>
+    <t>TRS.CONNECTOR.FUNC.0006</t>
+  </si>
+  <si>
+    <t>TRS.CONNECTOR.FUNC.0007</t>
+  </si>
+  <si>
+    <t>TRS.CONNECTOR.FUNC.0008</t>
+  </si>
+  <si>
+    <t>TRS.CONNECTOR.FUNC.0009</t>
+  </si>
+  <si>
+    <t>TRS.CONNECTOR.GEN.001</t>
+  </si>
+  <si>
+    <t>TRS.CONNECTOR.GEN.002</t>
+  </si>
+  <si>
+    <t>TRS.CONNECTOR.GEN.003</t>
+  </si>
+  <si>
+    <t>TRS.CONNECTOR.GEN.004</t>
   </si>
 </sst>
 </file>
@@ -692,7 +706,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -959,11 +973,69 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -977,9 +1049,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -991,13 +1060,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1005,51 +1068,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1071,12 +1095,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1085,6 +1103,58 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1407,453 +1477,552 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B18"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="24" customWidth="1"/>
+    <col min="2" max="2" width="68.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="25"/>
+      <c r="B3" s="26"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="25"/>
+      <c r="B4" s="26"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="25"/>
+      <c r="B5" s="26"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="25"/>
+      <c r="B6" s="26"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="25"/>
+      <c r="B7" s="26"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="25"/>
+      <c r="B8" s="26"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="25"/>
+      <c r="B9" s="26"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="25"/>
+      <c r="B10" s="26"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="25"/>
+      <c r="B11" s="26"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="25"/>
+      <c r="B12" s="26"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="25"/>
+      <c r="B13" s="26"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="25"/>
+      <c r="B14" s="26"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="25"/>
+      <c r="B15" s="26"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="25"/>
+      <c r="B16" s="26"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="25"/>
+      <c r="B17" s="26"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="25"/>
+      <c r="B18" s="26"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B17" sqref="B17"/>
+      <selection pane="bottomRight" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="48.85546875" style="12" customWidth="1"/>
+    <col min="1" max="1" width="35.42578125" style="38" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="79.140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="46.28515625" style="1" customWidth="1"/>
     <col min="5" max="5" width="17.28515625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="10" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="40" t="s">
+      <c r="D1" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="41" t="s">
-        <v>75</v>
-      </c>
-      <c r="F1" s="41" t="s">
-        <v>76</v>
+      <c r="E1" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="14" t="s">
+      <c r="A2" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="D2" s="34" t="s">
-        <v>66</v>
-      </c>
-      <c r="E2" s="35" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="36" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="40"/>
       <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" s="40" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="35"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="E3" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="32" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="B7" s="41" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="35"/>
+      <c r="B8" s="42"/>
+      <c r="C8" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="33" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="B11" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="33" t="s">
+        <v>74</v>
+      </c>
+      <c r="B12" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A13" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="B13" s="41" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A14" s="35"/>
+      <c r="B14" s="42"/>
+      <c r="C14" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" s="16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="B15" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" s="16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="35"/>
+      <c r="B16" s="42"/>
+      <c r="C16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="B17" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" s="16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="33" t="s">
+        <v>78</v>
+      </c>
+      <c r="B18" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" s="16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A19" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="B19" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19" s="16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" s="35"/>
+      <c r="B20" s="42"/>
+      <c r="C20" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" s="16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="34" t="s">
+        <v>80</v>
+      </c>
+      <c r="B21" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F21" s="16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="36"/>
+      <c r="B22" s="44"/>
+      <c r="C22" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22" s="16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="37"/>
+      <c r="B23" s="45"/>
+      <c r="C23" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="E4" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="32" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E5" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="32" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="19"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="E6" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" s="32" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="E7" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" s="32" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="24"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D8" s="25" t="s">
-        <v>72</v>
-      </c>
-      <c r="E8" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8" s="32" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="E9" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="F9" s="32" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E10" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10" s="32" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="E11" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="F11" s="32" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="E12" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="F12" s="32" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A13" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E13" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="F13" s="32" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" s="24"/>
-      <c r="B14" s="22"/>
-      <c r="C14" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="E14" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="F14" s="32" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="E15" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="F15" s="32" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="19"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="E16" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="F16" s="32" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="E17" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="F17" s="32" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="D18" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="E18" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="F18" s="32" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A19" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="B19" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E19" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="F19" s="32" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A20" s="19"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E20" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="F20" s="32" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="18" t="s">
+      <c r="D23" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E21" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="F21" s="32" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="27"/>
-      <c r="B22" s="20"/>
-      <c r="C22" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E22" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="F22" s="32" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="28"/>
-      <c r="B23" s="29"/>
-      <c r="C23" s="30" t="s">
-        <v>30</v>
-      </c>
-      <c r="D23" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="E23" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="F23" s="32" t="s">
-        <v>63</v>
+      <c r="E23" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F23" s="16" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final Update V1 delivery
</commit_message>
<xml_diff>
--- a/ABU test plan.xlsx
+++ b/ABU test plan.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="5940" windowWidth="19260" windowHeight="6000" activeTab="1"/>
+    <workbookView xWindow="-15" yWindow="5940" windowWidth="19260" windowHeight="6000"/>
   </bookViews>
   <sheets>
     <sheet name="Version" sheetId="3" r:id="rId1"/>
@@ -1111,8 +1111,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1120,18 +1118,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -1141,13 +1127,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1156,6 +1148,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1479,8 +1479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1490,10 +1490,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="44" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="45" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1571,6 +1571,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1578,7 +1579,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -1587,7 +1588,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.42578125" style="38" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.42578125" style="32" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="48.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="79.140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="46.28515625" style="1" customWidth="1"/>
@@ -1596,7 +1597,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="21" t="s">
@@ -1616,10 +1617,10 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="33" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="11" t="s">
@@ -1636,10 +1637,10 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="B3" s="40"/>
+      <c r="B3" s="34"/>
       <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
@@ -1654,10 +1655,10 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="34" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -1674,10 +1675,10 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="38" t="s">
         <v>69</v>
       </c>
-      <c r="B5" s="41" t="s">
+      <c r="B5" s="36" t="s">
         <v>45</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -1694,8 +1695,8 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="35"/>
-      <c r="B6" s="42"/>
+      <c r="A6" s="39"/>
+      <c r="B6" s="37"/>
       <c r="C6" s="2" t="s">
         <v>58</v>
       </c>
@@ -1710,10 +1711,10 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="34" t="s">
+      <c r="A7" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="B7" s="41" t="s">
+      <c r="B7" s="36" t="s">
         <v>41</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -1730,8 +1731,8 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="35"/>
-      <c r="B8" s="42"/>
+      <c r="A8" s="39"/>
+      <c r="B8" s="37"/>
       <c r="C8" s="2" t="s">
         <v>56</v>
       </c>
@@ -1746,10 +1747,10 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="33" t="s">
+      <c r="A9" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="34" t="s">
         <v>39</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -1766,10 +1767,10 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="33" t="s">
+      <c r="A10" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="B10" s="40" t="s">
+      <c r="B10" s="34" t="s">
         <v>34</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -1786,10 +1787,10 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="33" t="s">
+      <c r="A11" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="B11" s="40" t="s">
+      <c r="B11" s="34" t="s">
         <v>33</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -1806,10 +1807,10 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="33" t="s">
+      <c r="A12" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="B12" s="40" t="s">
+      <c r="B12" s="34" t="s">
         <v>32</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -1826,10 +1827,10 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A13" s="34" t="s">
+      <c r="A13" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="B13" s="41" t="s">
+      <c r="B13" s="36" t="s">
         <v>28</v>
       </c>
       <c r="C13" s="10" t="s">
@@ -1846,8 +1847,8 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" s="35"/>
-      <c r="B14" s="42"/>
+      <c r="A14" s="39"/>
+      <c r="B14" s="37"/>
       <c r="C14" s="10" t="s">
         <v>49</v>
       </c>
@@ -1862,10 +1863,10 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="34" t="s">
+      <c r="A15" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="B15" s="41" t="s">
+      <c r="B15" s="36" t="s">
         <v>26</v>
       </c>
       <c r="C15" s="10" t="s">
@@ -1882,8 +1883,8 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="35"/>
-      <c r="B16" s="42"/>
+      <c r="A16" s="39"/>
+      <c r="B16" s="37"/>
       <c r="C16" s="2" t="s">
         <v>30</v>
       </c>
@@ -1898,10 +1899,10 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="33" t="s">
+      <c r="A17" s="31" t="s">
         <v>77</v>
       </c>
-      <c r="B17" s="40" t="s">
+      <c r="B17" s="34" t="s">
         <v>5</v>
       </c>
       <c r="C17" s="8" t="s">
@@ -1918,10 +1919,10 @@
       </c>
     </row>
     <row r="18" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="33" t="s">
+      <c r="A18" s="31" t="s">
         <v>78</v>
       </c>
-      <c r="B18" s="43" t="s">
+      <c r="B18" s="35" t="s">
         <v>9</v>
       </c>
       <c r="C18" s="8" t="s">
@@ -1938,10 +1939,10 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A19" s="34" t="s">
+      <c r="A19" s="38" t="s">
         <v>79</v>
       </c>
-      <c r="B19" s="41" t="s">
+      <c r="B19" s="36" t="s">
         <v>10</v>
       </c>
       <c r="C19" s="10" t="s">
@@ -1958,8 +1959,8 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A20" s="35"/>
-      <c r="B20" s="42"/>
+      <c r="A20" s="39"/>
+      <c r="B20" s="37"/>
       <c r="C20" s="2" t="s">
         <v>18</v>
       </c>
@@ -1974,10 +1975,10 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="34" t="s">
+      <c r="A21" s="38" t="s">
         <v>80</v>
       </c>
-      <c r="B21" s="41" t="s">
+      <c r="B21" s="36" t="s">
         <v>11</v>
       </c>
       <c r="C21" s="10" t="s">
@@ -1994,8 +1995,8 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="36"/>
-      <c r="B22" s="44"/>
+      <c r="A22" s="42"/>
+      <c r="B22" s="40"/>
       <c r="C22" s="10" t="s">
         <v>13</v>
       </c>
@@ -2010,8 +2011,8 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="37"/>
-      <c r="B23" s="45"/>
+      <c r="A23" s="43"/>
+      <c r="B23" s="41"/>
       <c r="C23" s="14" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
test plan: added new test-cases to be implemented
</commit_message>
<xml_diff>
--- a/ABU test plan.xlsx
+++ b/ABU test plan.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="5940" windowWidth="19260" windowHeight="6000"/>
+    <workbookView xWindow="-15" yWindow="5940" windowWidth="19260" windowHeight="6000" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Version" sheetId="3" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="96">
   <si>
     <t>Requirements</t>
   </si>
@@ -675,6 +675,52 @@
   </si>
   <si>
     <t>TRS.CONNECTOR.GEN.004</t>
+  </si>
+  <si>
+    <t>1.1</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>4/5/2018</t>
+  </si>
+  <si>
+    <t>3/2/2018</t>
+  </si>
+  <si>
+    <t>-added new test-cases (to cover MSI ports connection)</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>CST</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Check the tool behavior in case of arxml not well formed</t>
+  </si>
+  <si>
+    <t>Provide to the tool one ".arxml" file that is not correct (tags not properly closed, multiple roots, etc)</t>
+  </si>
+  <si>
+    <t>- check that the output arxml file is not produced
+- check the log for the corresponding error</t>
+  </si>
+  <si>
+    <t>not done</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>Check the tool behavior in case of dico not well formed</t>
+  </si>
+  <si>
+    <t>Provide to the tool one ".dico" file that is not correct (tags not properly closed, multiple roots, etc)</t>
   </si>
 </sst>
 </file>
@@ -706,7 +752,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="34">
     <border>
       <left/>
       <right/>
@@ -1031,11 +1077,85 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1130,6 +1250,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1154,13 +1276,238 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="24">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1477,97 +1824,150 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="A1:B1"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="24" customWidth="1"/>
-    <col min="2" max="2" width="68.42578125" customWidth="1"/>
+    <col min="1" max="2" width="9.140625" style="24" customWidth="1"/>
+    <col min="3" max="3" width="68.42578125" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="44" t="s">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="36" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="46" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" s="37" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1" s="48" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" s="28" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="25"/>
-      <c r="B3" s="26"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D2" s="27" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3" s="47" t="s">
+        <v>85</v>
+      </c>
+      <c r="D3" s="27" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="25"/>
-      <c r="B4" s="26"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="25"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="25"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="25"/>
-      <c r="B5" s="26"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" s="25"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="25"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="25"/>
-      <c r="B6" s="26"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" s="25"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="25"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="25"/>
-      <c r="B7" s="26"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7" s="25"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="25"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="25"/>
-      <c r="B8" s="26"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8" s="25"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="25"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="25"/>
-      <c r="B9" s="26"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" s="25"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="25"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="25"/>
-      <c r="B10" s="26"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B10" s="25"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="25"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="25"/>
-      <c r="B11" s="26"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B11" s="25"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="25"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="25"/>
-      <c r="B12" s="26"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B12" s="25"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="25"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="25"/>
-      <c r="B13" s="26"/>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B13" s="25"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="25"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="25"/>
-      <c r="B14" s="26"/>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B14" s="25"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="25"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="25"/>
-      <c r="B15" s="26"/>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B15" s="25"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="25"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="25"/>
-      <c r="B16" s="26"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B16" s="25"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="25"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="25"/>
-      <c r="B17" s="26"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="25"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="25"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="25"/>
-      <c r="B18" s="26"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="25"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1577,13 +1977,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomRight" activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1675,10 +2075,10 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="40" t="s">
         <v>69</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="38" t="s">
         <v>45</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -1695,8 +2095,8 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="39"/>
-      <c r="B6" s="37"/>
+      <c r="A6" s="41"/>
+      <c r="B6" s="39"/>
       <c r="C6" s="2" t="s">
         <v>58</v>
       </c>
@@ -1711,10 +2111,10 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="38" t="s">
+      <c r="A7" s="40" t="s">
         <v>70</v>
       </c>
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="38" t="s">
         <v>41</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -1731,8 +2131,8 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="39"/>
-      <c r="B8" s="37"/>
+      <c r="A8" s="41"/>
+      <c r="B8" s="39"/>
       <c r="C8" s="2" t="s">
         <v>56</v>
       </c>
@@ -1827,10 +2227,10 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A13" s="38" t="s">
+      <c r="A13" s="40" t="s">
         <v>75</v>
       </c>
-      <c r="B13" s="36" t="s">
+      <c r="B13" s="38" t="s">
         <v>28</v>
       </c>
       <c r="C13" s="10" t="s">
@@ -1847,8 +2247,8 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" s="39"/>
-      <c r="B14" s="37"/>
+      <c r="A14" s="41"/>
+      <c r="B14" s="39"/>
       <c r="C14" s="10" t="s">
         <v>49</v>
       </c>
@@ -1863,10 +2263,10 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="38" t="s">
+      <c r="A15" s="40" t="s">
         <v>76</v>
       </c>
-      <c r="B15" s="36" t="s">
+      <c r="B15" s="38" t="s">
         <v>26</v>
       </c>
       <c r="C15" s="10" t="s">
@@ -1883,8 +2283,8 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="39"/>
-      <c r="B16" s="37"/>
+      <c r="A16" s="41"/>
+      <c r="B16" s="39"/>
       <c r="C16" s="2" t="s">
         <v>30</v>
       </c>
@@ -1939,10 +2339,10 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A19" s="38" t="s">
+      <c r="A19" s="40" t="s">
         <v>79</v>
       </c>
-      <c r="B19" s="36" t="s">
+      <c r="B19" s="38" t="s">
         <v>10</v>
       </c>
       <c r="C19" s="10" t="s">
@@ -1959,8 +2359,8 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A20" s="39"/>
-      <c r="B20" s="37"/>
+      <c r="A20" s="41"/>
+      <c r="B20" s="39"/>
       <c r="C20" s="2" t="s">
         <v>18</v>
       </c>
@@ -1975,10 +2375,10 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="38" t="s">
+      <c r="A21" s="40" t="s">
         <v>80</v>
       </c>
-      <c r="B21" s="36" t="s">
+      <c r="B21" s="38" t="s">
         <v>11</v>
       </c>
       <c r="C21" s="10" t="s">
@@ -1995,8 +2395,8 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="42"/>
-      <c r="B22" s="40"/>
+      <c r="A22" s="44"/>
+      <c r="B22" s="42"/>
       <c r="C22" s="10" t="s">
         <v>13</v>
       </c>
@@ -2011,8 +2411,8 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="43"/>
-      <c r="B23" s="41"/>
+      <c r="A23" s="45"/>
+      <c r="B23" s="43"/>
       <c r="C23" s="14" t="s">
         <v>15</v>
       </c>
@@ -2024,6 +2424,46 @@
       </c>
       <c r="F23" s="16" t="s">
         <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="49" t="s">
+        <v>88</v>
+      </c>
+      <c r="B24" s="50" t="s">
+        <v>89</v>
+      </c>
+      <c r="C24" s="51" t="s">
+        <v>90</v>
+      </c>
+      <c r="D24" s="52" t="s">
+        <v>91</v>
+      </c>
+      <c r="E24" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="F24" s="20" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="53" t="s">
+        <v>88</v>
+      </c>
+      <c r="B25" s="54" t="s">
+        <v>94</v>
+      </c>
+      <c r="C25" s="55" t="s">
+        <v>95</v>
+      </c>
+      <c r="D25" s="56" t="s">
+        <v>91</v>
+      </c>
+      <c r="E25" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="F25" s="20" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -2042,30 +2482,75 @@
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="A7:A8"/>
   </mergeCells>
-  <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+  <conditionalFormatting sqref="E1:E23 E26:E1048576">
+    <cfRule type="cellIs" dxfId="23" priority="13" operator="equal">
       <formula>"done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="14" operator="equal">
       <formula>"not done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F23">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="12" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F23">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="11" operator="equal">
       <formula>"YES"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E23">
+  <conditionalFormatting sqref="E24">
+    <cfRule type="cellIs" dxfId="19" priority="9" operator="equal">
+      <formula>"done"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="10" operator="equal">
+      <formula>"not done"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F24">
+    <cfRule type="cellIs" dxfId="15" priority="6" operator="equal">
+      <formula>"N/A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="8" operator="equal">
+      <formula>"NO"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F24">
+    <cfRule type="cellIs" dxfId="11" priority="7" operator="equal">
+      <formula>"YES"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="cellIs" dxfId="9" priority="4" operator="equal">
+      <formula>"done"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
+      <formula>"not done"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F25">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+      <formula>"N/A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+      <formula>"NO"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F25">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>"YES"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E25">
       <formula1>"done, not done"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F23">
       <formula1>"YES, NO"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F24:F25">
+      <formula1>"YES, NO, N/A"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>